<commit_message>
filtros de busqueda para copras
</commit_message>
<xml_diff>
--- a/dev_docs/scrum/fastorder - estimacion y entregas.xlsx
+++ b/dev_docs/scrum/fastorder - estimacion y entregas.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="75" windowWidth="16515" windowHeight="7995"/>
@@ -10,12 +10,12 @@
     <sheet name="Tareas" sheetId="1" r:id="rId1"/>
     <sheet name="Entrega 2" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t>Tiempo</t>
   </si>
@@ -158,24 +158,9 @@
     <t>Seleccionar e instalar un software para el api y cookbook del proyecto</t>
   </si>
   <si>
-    <t>Como encargado de compras, quiero saber qué comprar, cuanto, cuando y a quien.</t>
-  </si>
-  <si>
     <t>Como encargado de compras, quiero saber hacia dónde enviar lo que compré.</t>
   </si>
   <si>
-    <t>Hacer reporte con los pedidos de cada almacén</t>
-  </si>
-  <si>
-    <t>Hacer reporte con los pedidos de todos los almacenes (pedido concentrado)</t>
-  </si>
-  <si>
-    <t>Hacer reporte con el pedido concentrado, separado por el proveedor que surte cada producto</t>
-  </si>
-  <si>
-    <t>crear boton para precargar pedidos internos del proveedor seleccionado.</t>
-  </si>
-  <si>
     <t>Como encargado de compras, quiero hacer listas de compras (orden de compra).</t>
   </si>
   <si>
@@ -185,12 +170,6 @@
     <t>crear funcion para hacer ordenes de compras por proveedor.</t>
   </si>
   <si>
-    <t>Como encargado de compras, quiero registrar las compras.</t>
-  </si>
-  <si>
-    <t>Crear catálogo de compra</t>
-  </si>
-  <si>
     <t>Relacionar los pedidos internos con la compra</t>
   </si>
   <si>
@@ -237,13 +216,70 @@
   </si>
   <si>
     <t>crear reporte de existencias por almacén y concetrada por articulos</t>
+  </si>
+  <si>
+    <t>Como encargado de compras, quiero un reporte con lo que pidió cada uno de los almacenes.</t>
+  </si>
+  <si>
+    <t>Como encargado de compras, quiero un reporte con los pedidos concentrados por artículo.</t>
+  </si>
+  <si>
+    <t>Hacer reporte de pedidos por almacen</t>
+  </si>
+  <si>
+    <t>Hacer reporte concentrado por articulo</t>
+  </si>
+  <si>
+    <t>Como encargado de compras, quiero que el sistema mantenga una relación de los artículos que maneja cada proveedor, y en el caso de los artículos que son manejados por varios proveedores, manejar prioridad.</t>
+  </si>
+  <si>
+    <t>Hacer catálogo proveedores</t>
+  </si>
+  <si>
+    <t>Hacer catálogo listas de articulos del proveedor.</t>
+  </si>
+  <si>
+    <t>relacionar compra con una o mas ordenes de compra (detalle contra detalle)</t>
+  </si>
+  <si>
+    <t>headers busqueda: serie - folio, proveedor, fecha, estado, docto, sub, IVA(impuesto1), total</t>
+  </si>
+  <si>
+    <t>filtros: fecha i,fecha f, folio i, folio f, serie, prov, almacen</t>
+  </si>
+  <si>
+    <t>mostrar ordenes de compra pendientes</t>
+  </si>
+  <si>
+    <t>mostrar una ventana con las ordenes (del proveedor seleccionado) pendientes por surtir y permitir selección multiple</t>
+  </si>
+  <si>
+    <t>cargar artículo usando su presentacion.</t>
+  </si>
+  <si>
+    <t>mostrar en una lista, los articulos de las ordenes seleccionadas, no acumulados</t>
+  </si>
+  <si>
+    <t>permitir agregar la lista de articulos a la compra (anexar) cantidad = Cant Pendiente Orden Compra</t>
+  </si>
+  <si>
+    <t>Como encargado de compras, quiero un reporte con los pedidos concentrados pero separados por el proveedor de los artículos.</t>
+  </si>
+  <si>
+    <t>Imprimir lista de articulos del proveedor</t>
+  </si>
+  <si>
+    <t>hacer pantalla para priorizar articulos por proveedor</t>
+  </si>
+  <si>
+    <t>reporte</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -311,6 +347,17 @@
       <name val="Cambria"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -344,7 +391,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -368,34 +415,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -699,10 +753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K98"/>
+  <dimension ref="A1:K110"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72:I72"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A86" zoomScale="110" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="B88" sqref="B88:I88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,12 +768,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -733,48 +787,48 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <f>SUM(B9:B102)</f>
-        <v>69.5</v>
+        <f>SUM(B9:B114)</f>
+        <v>73</v>
       </c>
       <c r="E3" t="s">
         <v>20</v>
       </c>
       <c r="F3">
         <f>D3*400</f>
-        <v>27800</v>
+        <v>29200</v>
       </c>
       <c r="G3">
         <f>F3-18000</f>
-        <v>9800</v>
+        <v>11200</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="14"/>
+      <c r="C6" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="13"/>
     </row>
     <row r="8" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>0.5</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -798,7 +852,7 @@
         <v>0.5</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="18" x14ac:dyDescent="0.25">
@@ -812,16 +866,16 @@
       <c r="I13" s="7"/>
     </row>
     <row r="14" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15">
@@ -837,23 +891,23 @@
       <c r="D17" s="8"/>
     </row>
     <row r="18" spans="2:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
+      <c r="B18" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="5">
         <v>2</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D19" s="10"/>
     </row>
@@ -862,7 +916,7 @@
         <v>2</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D20" s="8"/>
     </row>
@@ -872,23 +926,23 @@
       <c r="D21" s="8"/>
     </row>
     <row r="22" spans="2:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
+      <c r="B22" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="5">
         <v>2</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D23" s="8"/>
     </row>
@@ -898,16 +952,16 @@
       <c r="D24" s="8"/>
     </row>
     <row r="25" spans="2:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
+      <c r="B25" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26">
@@ -918,56 +972,56 @@
       </c>
     </row>
     <row r="28" spans="2:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
+      <c r="B28" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="2:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="11"/>
+      <c r="B31" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="11" t="s">
+      <c r="B35" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="11"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36">
@@ -986,30 +1040,30 @@
       </c>
     </row>
     <row r="39" spans="2:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="11" t="s">
+      <c r="B39" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
-      <c r="I39" s="11"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="15"/>
     </row>
     <row r="40" spans="2:9" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="3">
         <v>0.5</v>
       </c>
-      <c r="C40" s="13" t="s">
+      <c r="C40" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="13"/>
-      <c r="I40" s="13"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="16"/>
+      <c r="H40" s="16"/>
+      <c r="I40" s="16"/>
     </row>
     <row r="41" spans="2:9" ht="18" x14ac:dyDescent="0.25">
       <c r="B41">
@@ -1024,7 +1078,7 @@
         <v>0.5</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="2:9" ht="18" x14ac:dyDescent="0.25">
@@ -1039,16 +1093,16 @@
       <c r="C44" s="4"/>
     </row>
     <row r="45" spans="2:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="11" t="s">
+      <c r="B45" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C45" s="11"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="11"/>
-      <c r="H45" s="11"/>
-      <c r="I45" s="11"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="15"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="15"/>
+      <c r="I45" s="15"/>
     </row>
     <row r="46" spans="2:9" ht="18" x14ac:dyDescent="0.25">
       <c r="B46">
@@ -1062,15 +1116,15 @@
       <c r="B47">
         <v>2</v>
       </c>
-      <c r="C47" s="13" t="s">
+      <c r="C47" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D47" s="13"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="13"/>
-      <c r="H47" s="13"/>
-      <c r="I47" s="13"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
+      <c r="H47" s="16"/>
+      <c r="I47" s="16"/>
     </row>
     <row r="48" spans="2:9" ht="18" x14ac:dyDescent="0.25">
       <c r="B48">
@@ -1084,15 +1138,15 @@
       <c r="B49" s="3">
         <v>1.5</v>
       </c>
-      <c r="C49" s="16" t="s">
+      <c r="C49" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D49" s="16"/>
-      <c r="E49" s="16"/>
-      <c r="F49" s="16"/>
-      <c r="G49" s="16"/>
-      <c r="H49" s="16"/>
-      <c r="I49" s="16"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="21"/>
+      <c r="H49" s="21"/>
+      <c r="I49" s="21"/>
     </row>
     <row r="50" spans="2:9" ht="18" x14ac:dyDescent="0.25">
       <c r="C50" s="4"/>
@@ -1101,16 +1155,16 @@
       <c r="C51" s="4"/>
     </row>
     <row r="52" spans="2:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="12" t="s">
+      <c r="B52" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C52" s="12"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="12"/>
-      <c r="F52" s="12"/>
-      <c r="G52" s="12"/>
-      <c r="H52" s="12"/>
-      <c r="I52" s="12"/>
+      <c r="C52" s="20"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="20"/>
+      <c r="H52" s="20"/>
+      <c r="I52" s="20"/>
     </row>
     <row r="53" spans="2:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53">
@@ -1220,74 +1274,64 @@
         <v>34</v>
       </c>
     </row>
-    <row r="72" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C72" s="17"/>
-      <c r="D72" s="17"/>
-      <c r="E72" s="17"/>
-      <c r="F72" s="17"/>
-      <c r="G72" s="17"/>
-      <c r="H72" s="17"/>
-      <c r="I72" s="17"/>
-    </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B73">
-        <v>1</v>
-      </c>
-      <c r="C73" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B74">
-        <v>1</v>
-      </c>
-      <c r="C74" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="75" spans="2:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C70" s="17"/>
+      <c r="D70" s="17"/>
+      <c r="E70" s="17"/>
+      <c r="F70" s="17"/>
+      <c r="G70" s="17"/>
+      <c r="H70" s="17"/>
+      <c r="I70" s="17"/>
+    </row>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B71">
+        <v>1</v>
+      </c>
+      <c r="C71" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="74" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C74" s="17"/>
+      <c r="D74" s="17"/>
+      <c r="E74" s="17"/>
+      <c r="F74" s="17"/>
+      <c r="G74" s="17"/>
+      <c r="H74" s="17"/>
+      <c r="I74" s="17"/>
+    </row>
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B75">
-        <v>2</v>
-      </c>
-      <c r="C75" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="D75" s="20"/>
-      <c r="E75" s="20"/>
-      <c r="F75" s="20"/>
-      <c r="G75" s="20"/>
-      <c r="H75" s="20"/>
-      <c r="I75" s="20"/>
-    </row>
-    <row r="77" spans="2:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="B77" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="C77" s="17"/>
-      <c r="D77" s="17"/>
-      <c r="E77" s="17"/>
-      <c r="F77" s="17"/>
-      <c r="G77" s="17"/>
-      <c r="H77" s="17"/>
-      <c r="I77" s="17"/>
-    </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B78">
-        <v>2</v>
-      </c>
-      <c r="C78" t="s">
-        <v>42</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C75" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="78" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B78" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C78" s="17"/>
+      <c r="D78" s="17"/>
+      <c r="E78" s="17"/>
+      <c r="F78" s="17"/>
+      <c r="G78" s="17"/>
+      <c r="H78" s="17"/>
+      <c r="I78" s="17"/>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B79">
         <v>1</v>
       </c>
       <c r="C79" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
     </row>
     <row r="80" spans="2:9" x14ac:dyDescent="0.25">
@@ -1295,75 +1339,206 @@
         <v>1.5</v>
       </c>
       <c r="C80" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="83" spans="2:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="C83" s="17"/>
-      <c r="D83" s="17"/>
-      <c r="E83" s="17"/>
-      <c r="F83" s="17"/>
-      <c r="G83" s="17"/>
-      <c r="H83" s="17"/>
-      <c r="I83" s="17"/>
-    </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B84">
-        <v>2</v>
-      </c>
-      <c r="C84" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="89" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B89" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B81">
+        <v>1</v>
+      </c>
+      <c r="C81" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D81" s="22"/>
+      <c r="E81" s="22"/>
+      <c r="F81" s="22"/>
+      <c r="G81" s="22"/>
+      <c r="H81" s="22"/>
+      <c r="I81" s="22"/>
+    </row>
+    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B82">
+        <v>1</v>
+      </c>
+      <c r="C82" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="D82" s="22"/>
+      <c r="E82" s="22"/>
+      <c r="F82" s="22"/>
+      <c r="G82" s="22"/>
+      <c r="H82" s="22"/>
+      <c r="I82" s="22"/>
+    </row>
+    <row r="84" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B84" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C84" s="17"/>
+      <c r="D84" s="17"/>
+      <c r="E84" s="17"/>
+      <c r="F84" s="17"/>
+      <c r="G84" s="17"/>
+      <c r="H84" s="17"/>
+      <c r="I84" s="17"/>
+    </row>
+    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B85">
+        <v>1</v>
+      </c>
+      <c r="C85" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="88" spans="2:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B88" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C89" s="17"/>
-      <c r="D89" s="17"/>
-      <c r="E89" s="17"/>
-      <c r="F89" s="17"/>
-      <c r="G89" s="17"/>
-      <c r="H89" s="17"/>
-      <c r="I89" s="17"/>
-    </row>
-    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B90">
+      <c r="C88" s="17"/>
+      <c r="D88" s="17"/>
+      <c r="E88" s="17"/>
+      <c r="F88" s="17"/>
+      <c r="G88" s="17"/>
+      <c r="H88" s="17"/>
+      <c r="I88" s="17"/>
+    </row>
+    <row r="89" spans="2:9" s="11" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B89" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="C89" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="D89" s="23"/>
+      <c r="E89" s="23"/>
+      <c r="F89" s="23"/>
+      <c r="G89" s="23"/>
+      <c r="H89" s="23"/>
+      <c r="I89" s="12"/>
+    </row>
+    <row r="90" spans="2:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B90" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="C90" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="D90" s="23"/>
+      <c r="E90" s="23"/>
+      <c r="F90" s="23"/>
+      <c r="G90" s="23"/>
+      <c r="H90" s="23"/>
+      <c r="I90" s="23"/>
+    </row>
+    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B91">
+        <v>1</v>
+      </c>
+      <c r="C91" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B92">
+        <v>0.5</v>
+      </c>
+      <c r="C92" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B93">
+        <v>1</v>
+      </c>
+      <c r="C93" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="94" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B94">
+        <v>1</v>
+      </c>
+      <c r="C94" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="95" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B95">
+        <v>0.5</v>
+      </c>
+      <c r="C95" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="96" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B96">
+        <v>1.5</v>
+      </c>
+      <c r="C96" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="97" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C97" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="98" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C98" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="101" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B101" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C101" s="17"/>
+      <c r="D101" s="17"/>
+      <c r="E101" s="17"/>
+      <c r="F101" s="17"/>
+      <c r="G101" s="17"/>
+      <c r="H101" s="17"/>
+      <c r="I101" s="17"/>
+    </row>
+    <row r="102" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B102">
         <v>7</v>
       </c>
-      <c r="C90" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="94" spans="2:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="C94" s="18"/>
-      <c r="D94" s="18"/>
-      <c r="E94" s="18"/>
-      <c r="F94" s="18"/>
-      <c r="G94" s="18"/>
-      <c r="H94" s="18"/>
-      <c r="I94" s="18"/>
-    </row>
-    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D98" t="s">
-        <v>55</v>
+      <c r="C102" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="106" spans="2:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B106" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C106" s="18"/>
+      <c r="D106" s="18"/>
+      <c r="E106" s="18"/>
+      <c r="F106" s="18"/>
+      <c r="G106" s="18"/>
+      <c r="H106" s="18"/>
+      <c r="I106" s="18"/>
+    </row>
+    <row r="110" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D110" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="B83:I83"/>
-    <mergeCell ref="B89:I89"/>
-    <mergeCell ref="B94:I94"/>
-    <mergeCell ref="B77:I77"/>
-    <mergeCell ref="C75:I75"/>
+  <mergeCells count="31">
+    <mergeCell ref="B74:I74"/>
+    <mergeCell ref="B78:I78"/>
+    <mergeCell ref="B70:I70"/>
+    <mergeCell ref="B101:I101"/>
+    <mergeCell ref="B106:I106"/>
+    <mergeCell ref="C81:I81"/>
+    <mergeCell ref="C89:H89"/>
+    <mergeCell ref="C90:I90"/>
+    <mergeCell ref="B84:I84"/>
+    <mergeCell ref="C82:I82"/>
+    <mergeCell ref="B88:I88"/>
     <mergeCell ref="B66:I66"/>
-    <mergeCell ref="B72:I72"/>
     <mergeCell ref="B14:I14"/>
     <mergeCell ref="B62:I62"/>
     <mergeCell ref="C55:I55"/>
@@ -1371,12 +1546,12 @@
     <mergeCell ref="B28:I28"/>
     <mergeCell ref="B52:I52"/>
     <mergeCell ref="C40:I40"/>
+    <mergeCell ref="C49:I49"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="B39:I39"/>
     <mergeCell ref="B45:I45"/>
     <mergeCell ref="C47:I47"/>
-    <mergeCell ref="C49:I49"/>
     <mergeCell ref="B35:I35"/>
     <mergeCell ref="B8:I8"/>
     <mergeCell ref="B18:I18"/>

</xml_diff>